<commit_message>
제2정규화 / TABLE 다수조회 / ROWNUM
</commit_message>
<xml_diff>
--- a/참고자료/매입매출테이블명세(2018-12-20).xlsx
+++ b/참고자료/매입매출테이블명세(2018-12-20).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="매입매출장" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="상품매입매출" sheetId="2" r:id="rId3"/>
     <sheet name="거래처정보" sheetId="6" r:id="rId4"/>
     <sheet name="상품정보" sheetId="7" r:id="rId5"/>
+    <sheet name="상품정보 (2)" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="259">
   <si>
     <t>매입/매출 관리대장</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -992,6 +993,50 @@
   </si>
   <si>
     <t>C_NAME</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열(9)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>매입단가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>매출단가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>숫자</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_IPRICE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_OPRICE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_CODE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_NAME</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBL_PRODUCT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR(9)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUMBER</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1463,6 +1508,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1470,9 +1518,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1814,12 +1859,12 @@
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:20" ht="21" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
       <c r="I2" s="10"/>
@@ -17087,7 +17132,7 @@
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A12" s="31"/>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="45" t="s">
         <v>221</v>
       </c>
       <c r="C12" s="37" t="s">
@@ -17347,7 +17392,7 @@
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A12" s="31"/>
-      <c r="B12" s="48"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
@@ -17445,8 +17490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:G5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -17590,7 +17635,7 @@
     </row>
     <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A12" s="31"/>
-      <c r="B12" s="48"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
@@ -17682,4 +17727,264 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.25" hidden="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="G5" s="38"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="31"/>
+      <c r="B6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A7" s="31"/>
+      <c r="B7" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A8" s="31"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="31"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A10" s="31"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+    </row>
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A11" s="31"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A12" s="31"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="31"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="31"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="31"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="31"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="31"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="31"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="31"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="34"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>